<commit_message>
Añadida la carpeta de test_results
</commit_message>
<xml_diff>
--- a/study_documents/parroquias/std_parroquias.xlsx
+++ b/study_documents/parroquias/std_parroquias.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Open-ELEC\src\open_elec\data\Codigos_estandar\parroquias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ELECU\study_documents\parroquias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{064BF646-FA0C-46F8-A273-3E97218351DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F7ECB3-8551-4915-A4C9-2E903284B438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="std_parroquias" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9373" uniqueCount="4267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9436" uniqueCount="4267">
   <si>
     <t>PROVINCIA_CODIGO</t>
   </si>
@@ -12826,7 +12827,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -12963,7 +12964,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13143,8 +13144,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -13259,6 +13272,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -13304,8 +13354,35 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -13364,20 +13441,86 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B546E19C-E11A-2999-96E6-5A9868B0CDFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="5381625" cy="3629025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G1048576" totalsRowShown="0">
-  <autoFilter ref="A1:G1048576"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:G1048576" totalsRowShown="0">
+  <autoFilter ref="A1:G1048576" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1048576">
     <sortCondition ref="E1:E1048576"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="PROVINCIA_CODIGO"/>
-    <tableColumn id="2" name="NOMBRE_PROVINCIA"/>
-    <tableColumn id="3" name="CANTON_CODIGO"/>
-    <tableColumn id="4" name="CANTON_NOMBRE"/>
-    <tableColumn id="5" name="PARROQUIA_CODIGO_OLD"/>
-    <tableColumn id="6" name="PARROQUIA_CODIGO"/>
-    <tableColumn id="7" name="PARROQUIA_NOMBRE"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PROVINCIA_CODIGO"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NOMBRE_PROVINCIA"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CANTON_CODIGO"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CANTON_NOMBRE"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="PARROQUIA_CODIGO_OLD"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PARROQUIA_CODIGO"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="PARROQUIA_NOMBRE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13699,11 +13842,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1342"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O1342"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:Q14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13715,9 +13858,16 @@
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" customWidth="1"/>
     <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13739,8 +13889,29 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2319</v>
       </c>
@@ -13762,8 +13933,29 @@
       <c r="G2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="4" t="s">
+        <v>2319</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>2320</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>2515</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>2516</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>2523</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>2524</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1704</v>
       </c>
@@ -13785,8 +13977,29 @@
       <c r="G3" t="s">
         <v>1759</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="7" t="s">
+        <v>1704</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>1705</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>1755</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>1756</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>1757</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>1758</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1855</v>
       </c>
@@ -13808,8 +14021,29 @@
       <c r="G4" t="s">
         <v>2064</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="4" t="s">
+        <v>1855</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>1856</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>2037</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>2038</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>2062</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>2063</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -13831,8 +14065,29 @@
       <c r="G5" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1222</v>
       </c>
@@ -13854,8 +14109,29 @@
       <c r="G6" t="s">
         <v>1332</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="4" t="s">
+        <v>1222</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>1223</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>1326</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>1327</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>1330</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3424</v>
       </c>
@@ -13877,8 +14153,29 @@
       <c r="G7" t="s">
         <v>3465</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="7" t="s">
+        <v>3424</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>3425</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>3456</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>3457</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>3463</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>3464</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>3465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2807</v>
       </c>
@@ -13900,8 +14197,29 @@
       <c r="G8" t="s">
         <v>2832</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="4" t="s">
+        <v>2807</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>2808</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>2826</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>2827</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>2830</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>2831</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>2832</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2889</v>
       </c>
@@ -13923,8 +14241,29 @@
       <c r="G9" t="s">
         <v>2503</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="7" t="s">
+        <v>2889</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>2890</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>2908</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>2890</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>2912</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>2913</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2319</v>
       </c>
@@ -13947,7 +14286,7 @@
         <v>2503</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1855</v>
       </c>
@@ -13970,7 +14309,7 @@
         <v>2069</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1704</v>
       </c>
@@ -13993,7 +14332,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3581</v>
       </c>
@@ -14016,7 +14355,7 @@
         <v>3626</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2319</v>
       </c>
@@ -14039,7 +14378,7 @@
         <v>2405</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3696</v>
       </c>
@@ -14062,7 +14401,7 @@
         <v>3789</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>507</v>
       </c>
@@ -44526,4 +44865,19 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D41955-7428-4474-8184-2F1D20899924}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>